<commit_message>
eliminacion de archivos dobles
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Cambios/PTL_Solicitud Cambios.xlsx
+++ b/qualtcom/Organizacional/Cambios/PTL_Solicitud Cambios.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\escuela1\qualtcom\Organizacional\Cambios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="15480" windowHeight="8076" tabRatio="663"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="15480" windowHeight="8070" tabRatio="663"/>
   </bookViews>
   <sheets>
     <sheet name="Control de Cambios" sheetId="15" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="Ocupacion">[2]Parámetros!$B$22:$B$23</definedName>
     <definedName name="UEN">[3]Parámetros!$A$1:$A$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -40,7 +45,7 @@
     <author>innevo</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -451,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,6 +610,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFE6E6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,24 +751,30 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color indexed="23"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="23"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="hair">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,7 +868,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -861,9 +884,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -873,41 +893,54 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" xfId="84" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" xfId="84" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="10" xfId="84" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="11" xfId="84" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="11" xfId="84" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" xfId="84" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" xfId="84" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" xfId="84" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="11" xfId="84" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="87">
     <cellStyle name="20% - Accent1" xfId="1"/>
@@ -959,6 +992,7 @@
     <cellStyle name="Celda de comprobación" xfId="47" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="48" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="49"/>
+    <cellStyle name="Encabezado 1" xfId="78" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="50" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="51" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="52" builtinId="33" customBuiltin="1"/>
@@ -992,7 +1026,6 @@
     <cellStyle name="Texto explicativo" xfId="75" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Title" xfId="76"/>
     <cellStyle name="Título" xfId="77" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="78" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="79" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="80" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="81" builtinId="25" customBuiltin="1"/>
@@ -1003,6 +1036,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1559,273 +1595,273 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="67.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="79" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="256" width="11.44140625" style="1"/>
-    <col min="257" max="257" width="2.6640625" style="1" customWidth="1"/>
-    <col min="258" max="258" width="28.5546875" style="1" customWidth="1"/>
-    <col min="259" max="259" width="57.44140625" style="1" customWidth="1"/>
-    <col min="260" max="512" width="11.44140625" style="1"/>
-    <col min="513" max="513" width="2.6640625" style="1" customWidth="1"/>
-    <col min="514" max="514" width="28.5546875" style="1" customWidth="1"/>
-    <col min="515" max="515" width="57.44140625" style="1" customWidth="1"/>
-    <col min="516" max="768" width="11.44140625" style="1"/>
-    <col min="769" max="769" width="2.6640625" style="1" customWidth="1"/>
-    <col min="770" max="770" width="28.5546875" style="1" customWidth="1"/>
-    <col min="771" max="771" width="57.44140625" style="1" customWidth="1"/>
-    <col min="772" max="1024" width="11.44140625" style="1"/>
-    <col min="1025" max="1025" width="2.6640625" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="28.5546875" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="57.44140625" style="1" customWidth="1"/>
-    <col min="1028" max="1280" width="11.44140625" style="1"/>
-    <col min="1281" max="1281" width="2.6640625" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="28.5546875" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="57.44140625" style="1" customWidth="1"/>
-    <col min="1284" max="1536" width="11.44140625" style="1"/>
-    <col min="1537" max="1537" width="2.6640625" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="28.5546875" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="57.44140625" style="1" customWidth="1"/>
-    <col min="1540" max="1792" width="11.44140625" style="1"/>
-    <col min="1793" max="1793" width="2.6640625" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="28.5546875" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="57.44140625" style="1" customWidth="1"/>
-    <col min="1796" max="2048" width="11.44140625" style="1"/>
-    <col min="2049" max="2049" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="28.5546875" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="57.44140625" style="1" customWidth="1"/>
-    <col min="2052" max="2304" width="11.44140625" style="1"/>
-    <col min="2305" max="2305" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="28.5546875" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="57.44140625" style="1" customWidth="1"/>
-    <col min="2308" max="2560" width="11.44140625" style="1"/>
-    <col min="2561" max="2561" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="28.5546875" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="57.44140625" style="1" customWidth="1"/>
-    <col min="2564" max="2816" width="11.44140625" style="1"/>
-    <col min="2817" max="2817" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="28.5546875" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="57.44140625" style="1" customWidth="1"/>
-    <col min="2820" max="3072" width="11.44140625" style="1"/>
-    <col min="3073" max="3073" width="2.6640625" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="28.5546875" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="57.44140625" style="1" customWidth="1"/>
-    <col min="3076" max="3328" width="11.44140625" style="1"/>
-    <col min="3329" max="3329" width="2.6640625" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="28.5546875" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="57.44140625" style="1" customWidth="1"/>
-    <col min="3332" max="3584" width="11.44140625" style="1"/>
-    <col min="3585" max="3585" width="2.6640625" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="28.5546875" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="57.44140625" style="1" customWidth="1"/>
-    <col min="3588" max="3840" width="11.44140625" style="1"/>
-    <col min="3841" max="3841" width="2.6640625" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="28.5546875" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="57.44140625" style="1" customWidth="1"/>
-    <col min="3844" max="4096" width="11.44140625" style="1"/>
-    <col min="4097" max="4097" width="2.6640625" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="28.5546875" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="57.44140625" style="1" customWidth="1"/>
-    <col min="4100" max="4352" width="11.44140625" style="1"/>
-    <col min="4353" max="4353" width="2.6640625" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="28.5546875" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="57.44140625" style="1" customWidth="1"/>
-    <col min="4356" max="4608" width="11.44140625" style="1"/>
-    <col min="4609" max="4609" width="2.6640625" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="28.5546875" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="57.44140625" style="1" customWidth="1"/>
-    <col min="4612" max="4864" width="11.44140625" style="1"/>
-    <col min="4865" max="4865" width="2.6640625" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="28.5546875" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="57.44140625" style="1" customWidth="1"/>
-    <col min="4868" max="5120" width="11.44140625" style="1"/>
-    <col min="5121" max="5121" width="2.6640625" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="28.5546875" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="57.44140625" style="1" customWidth="1"/>
-    <col min="5124" max="5376" width="11.44140625" style="1"/>
-    <col min="5377" max="5377" width="2.6640625" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="28.5546875" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="57.44140625" style="1" customWidth="1"/>
-    <col min="5380" max="5632" width="11.44140625" style="1"/>
-    <col min="5633" max="5633" width="2.6640625" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="28.5546875" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="57.44140625" style="1" customWidth="1"/>
-    <col min="5636" max="5888" width="11.44140625" style="1"/>
-    <col min="5889" max="5889" width="2.6640625" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="28.5546875" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="57.44140625" style="1" customWidth="1"/>
-    <col min="5892" max="6144" width="11.44140625" style="1"/>
-    <col min="6145" max="6145" width="2.6640625" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="28.5546875" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="57.44140625" style="1" customWidth="1"/>
-    <col min="6148" max="6400" width="11.44140625" style="1"/>
-    <col min="6401" max="6401" width="2.6640625" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="28.5546875" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="57.44140625" style="1" customWidth="1"/>
-    <col min="6404" max="6656" width="11.44140625" style="1"/>
-    <col min="6657" max="6657" width="2.6640625" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="28.5546875" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="57.44140625" style="1" customWidth="1"/>
-    <col min="6660" max="6912" width="11.44140625" style="1"/>
-    <col min="6913" max="6913" width="2.6640625" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="28.5546875" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="57.44140625" style="1" customWidth="1"/>
-    <col min="6916" max="7168" width="11.44140625" style="1"/>
-    <col min="7169" max="7169" width="2.6640625" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="28.5546875" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="57.44140625" style="1" customWidth="1"/>
-    <col min="7172" max="7424" width="11.44140625" style="1"/>
-    <col min="7425" max="7425" width="2.6640625" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="28.5546875" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="57.44140625" style="1" customWidth="1"/>
-    <col min="7428" max="7680" width="11.44140625" style="1"/>
-    <col min="7681" max="7681" width="2.6640625" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="28.5546875" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="57.44140625" style="1" customWidth="1"/>
-    <col min="7684" max="7936" width="11.44140625" style="1"/>
-    <col min="7937" max="7937" width="2.6640625" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="28.5546875" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="57.44140625" style="1" customWidth="1"/>
-    <col min="7940" max="8192" width="11.44140625" style="1"/>
-    <col min="8193" max="8193" width="2.6640625" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="28.5546875" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="57.44140625" style="1" customWidth="1"/>
-    <col min="8196" max="8448" width="11.44140625" style="1"/>
-    <col min="8449" max="8449" width="2.6640625" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="28.5546875" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="57.44140625" style="1" customWidth="1"/>
-    <col min="8452" max="8704" width="11.44140625" style="1"/>
-    <col min="8705" max="8705" width="2.6640625" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="28.5546875" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="57.44140625" style="1" customWidth="1"/>
-    <col min="8708" max="8960" width="11.44140625" style="1"/>
-    <col min="8961" max="8961" width="2.6640625" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="28.5546875" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="57.44140625" style="1" customWidth="1"/>
-    <col min="8964" max="9216" width="11.44140625" style="1"/>
-    <col min="9217" max="9217" width="2.6640625" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="28.5546875" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="57.44140625" style="1" customWidth="1"/>
-    <col min="9220" max="9472" width="11.44140625" style="1"/>
-    <col min="9473" max="9473" width="2.6640625" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="28.5546875" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="57.44140625" style="1" customWidth="1"/>
-    <col min="9476" max="9728" width="11.44140625" style="1"/>
-    <col min="9729" max="9729" width="2.6640625" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="28.5546875" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="57.44140625" style="1" customWidth="1"/>
-    <col min="9732" max="9984" width="11.44140625" style="1"/>
-    <col min="9985" max="9985" width="2.6640625" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="28.5546875" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="57.44140625" style="1" customWidth="1"/>
-    <col min="9988" max="10240" width="11.44140625" style="1"/>
-    <col min="10241" max="10241" width="2.6640625" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="28.5546875" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="57.44140625" style="1" customWidth="1"/>
-    <col min="10244" max="10496" width="11.44140625" style="1"/>
-    <col min="10497" max="10497" width="2.6640625" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="28.5546875" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="57.44140625" style="1" customWidth="1"/>
-    <col min="10500" max="10752" width="11.44140625" style="1"/>
-    <col min="10753" max="10753" width="2.6640625" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="28.5546875" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="57.44140625" style="1" customWidth="1"/>
-    <col min="10756" max="11008" width="11.44140625" style="1"/>
-    <col min="11009" max="11009" width="2.6640625" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="28.5546875" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="57.44140625" style="1" customWidth="1"/>
-    <col min="11012" max="11264" width="11.44140625" style="1"/>
-    <col min="11265" max="11265" width="2.6640625" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="28.5546875" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="57.44140625" style="1" customWidth="1"/>
-    <col min="11268" max="11520" width="11.44140625" style="1"/>
-    <col min="11521" max="11521" width="2.6640625" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="28.5546875" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="57.44140625" style="1" customWidth="1"/>
-    <col min="11524" max="11776" width="11.44140625" style="1"/>
-    <col min="11777" max="11777" width="2.6640625" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="28.5546875" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="57.44140625" style="1" customWidth="1"/>
-    <col min="11780" max="12032" width="11.44140625" style="1"/>
-    <col min="12033" max="12033" width="2.6640625" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="28.5546875" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="57.44140625" style="1" customWidth="1"/>
-    <col min="12036" max="12288" width="11.44140625" style="1"/>
-    <col min="12289" max="12289" width="2.6640625" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="28.5546875" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="57.44140625" style="1" customWidth="1"/>
-    <col min="12292" max="12544" width="11.44140625" style="1"/>
-    <col min="12545" max="12545" width="2.6640625" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="28.5546875" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="57.44140625" style="1" customWidth="1"/>
-    <col min="12548" max="12800" width="11.44140625" style="1"/>
-    <col min="12801" max="12801" width="2.6640625" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="28.5546875" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="57.44140625" style="1" customWidth="1"/>
-    <col min="12804" max="13056" width="11.44140625" style="1"/>
-    <col min="13057" max="13057" width="2.6640625" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="28.5546875" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="57.44140625" style="1" customWidth="1"/>
-    <col min="13060" max="13312" width="11.44140625" style="1"/>
-    <col min="13313" max="13313" width="2.6640625" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="28.5546875" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="57.44140625" style="1" customWidth="1"/>
-    <col min="13316" max="13568" width="11.44140625" style="1"/>
-    <col min="13569" max="13569" width="2.6640625" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="28.5546875" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="57.44140625" style="1" customWidth="1"/>
-    <col min="13572" max="13824" width="11.44140625" style="1"/>
-    <col min="13825" max="13825" width="2.6640625" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="28.5546875" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="57.44140625" style="1" customWidth="1"/>
-    <col min="13828" max="14080" width="11.44140625" style="1"/>
-    <col min="14081" max="14081" width="2.6640625" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="28.5546875" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="57.44140625" style="1" customWidth="1"/>
-    <col min="14084" max="14336" width="11.44140625" style="1"/>
-    <col min="14337" max="14337" width="2.6640625" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="28.5546875" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="57.44140625" style="1" customWidth="1"/>
-    <col min="14340" max="14592" width="11.44140625" style="1"/>
-    <col min="14593" max="14593" width="2.6640625" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="28.5546875" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="57.44140625" style="1" customWidth="1"/>
-    <col min="14596" max="14848" width="11.44140625" style="1"/>
-    <col min="14849" max="14849" width="2.6640625" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="28.5546875" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="57.44140625" style="1" customWidth="1"/>
-    <col min="14852" max="15104" width="11.44140625" style="1"/>
-    <col min="15105" max="15105" width="2.6640625" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="28.5546875" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="57.44140625" style="1" customWidth="1"/>
-    <col min="15108" max="15360" width="11.44140625" style="1"/>
-    <col min="15361" max="15361" width="2.6640625" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="28.5546875" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="57.44140625" style="1" customWidth="1"/>
-    <col min="15364" max="15616" width="11.44140625" style="1"/>
-    <col min="15617" max="15617" width="2.6640625" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="28.5546875" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="57.44140625" style="1" customWidth="1"/>
-    <col min="15620" max="15872" width="11.44140625" style="1"/>
-    <col min="15873" max="15873" width="2.6640625" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="28.5546875" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="57.44140625" style="1" customWidth="1"/>
-    <col min="15876" max="16128" width="11.44140625" style="1"/>
-    <col min="16129" max="16129" width="2.6640625" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="28.5546875" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="57.44140625" style="1" customWidth="1"/>
-    <col min="16132" max="16384" width="11.44140625" style="1"/>
+    <col min="7" max="256" width="11.42578125" style="1"/>
+    <col min="257" max="257" width="2.7109375" style="1" customWidth="1"/>
+    <col min="258" max="258" width="28.5703125" style="1" customWidth="1"/>
+    <col min="259" max="259" width="57.42578125" style="1" customWidth="1"/>
+    <col min="260" max="512" width="11.42578125" style="1"/>
+    <col min="513" max="513" width="2.7109375" style="1" customWidth="1"/>
+    <col min="514" max="514" width="28.5703125" style="1" customWidth="1"/>
+    <col min="515" max="515" width="57.42578125" style="1" customWidth="1"/>
+    <col min="516" max="768" width="11.42578125" style="1"/>
+    <col min="769" max="769" width="2.7109375" style="1" customWidth="1"/>
+    <col min="770" max="770" width="28.5703125" style="1" customWidth="1"/>
+    <col min="771" max="771" width="57.42578125" style="1" customWidth="1"/>
+    <col min="772" max="1024" width="11.42578125" style="1"/>
+    <col min="1025" max="1025" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1026" max="1026" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="57.42578125" style="1" customWidth="1"/>
+    <col min="1028" max="1280" width="11.42578125" style="1"/>
+    <col min="1281" max="1281" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1282" max="1282" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="57.42578125" style="1" customWidth="1"/>
+    <col min="1284" max="1536" width="11.42578125" style="1"/>
+    <col min="1537" max="1537" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1538" max="1538" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="57.42578125" style="1" customWidth="1"/>
+    <col min="1540" max="1792" width="11.42578125" style="1"/>
+    <col min="1793" max="1793" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1794" max="1794" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="57.42578125" style="1" customWidth="1"/>
+    <col min="1796" max="2048" width="11.42578125" style="1"/>
+    <col min="2049" max="2049" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2050" max="2050" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="57.42578125" style="1" customWidth="1"/>
+    <col min="2052" max="2304" width="11.42578125" style="1"/>
+    <col min="2305" max="2305" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2306" max="2306" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="57.42578125" style="1" customWidth="1"/>
+    <col min="2308" max="2560" width="11.42578125" style="1"/>
+    <col min="2561" max="2561" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2562" max="2562" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="57.42578125" style="1" customWidth="1"/>
+    <col min="2564" max="2816" width="11.42578125" style="1"/>
+    <col min="2817" max="2817" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2818" max="2818" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="57.42578125" style="1" customWidth="1"/>
+    <col min="2820" max="3072" width="11.42578125" style="1"/>
+    <col min="3073" max="3073" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3074" max="3074" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="57.42578125" style="1" customWidth="1"/>
+    <col min="3076" max="3328" width="11.42578125" style="1"/>
+    <col min="3329" max="3329" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3330" max="3330" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="57.42578125" style="1" customWidth="1"/>
+    <col min="3332" max="3584" width="11.42578125" style="1"/>
+    <col min="3585" max="3585" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3586" max="3586" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="57.42578125" style="1" customWidth="1"/>
+    <col min="3588" max="3840" width="11.42578125" style="1"/>
+    <col min="3841" max="3841" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3842" max="3842" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="57.42578125" style="1" customWidth="1"/>
+    <col min="3844" max="4096" width="11.42578125" style="1"/>
+    <col min="4097" max="4097" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4098" max="4098" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="57.42578125" style="1" customWidth="1"/>
+    <col min="4100" max="4352" width="11.42578125" style="1"/>
+    <col min="4353" max="4353" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4354" max="4354" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="57.42578125" style="1" customWidth="1"/>
+    <col min="4356" max="4608" width="11.42578125" style="1"/>
+    <col min="4609" max="4609" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4610" max="4610" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="57.42578125" style="1" customWidth="1"/>
+    <col min="4612" max="4864" width="11.42578125" style="1"/>
+    <col min="4865" max="4865" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4866" max="4866" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="57.42578125" style="1" customWidth="1"/>
+    <col min="4868" max="5120" width="11.42578125" style="1"/>
+    <col min="5121" max="5121" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5122" max="5122" width="28.5703125" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="57.42578125" style="1" customWidth="1"/>
+    <col min="5124" max="5376" width="11.42578125" style="1"/>
+    <col min="5377" max="5377" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5378" max="5378" width="28.5703125" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="57.42578125" style="1" customWidth="1"/>
+    <col min="5380" max="5632" width="11.42578125" style="1"/>
+    <col min="5633" max="5633" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5634" max="5634" width="28.5703125" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="57.42578125" style="1" customWidth="1"/>
+    <col min="5636" max="5888" width="11.42578125" style="1"/>
+    <col min="5889" max="5889" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5890" max="5890" width="28.5703125" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="57.42578125" style="1" customWidth="1"/>
+    <col min="5892" max="6144" width="11.42578125" style="1"/>
+    <col min="6145" max="6145" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6146" max="6146" width="28.5703125" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="57.42578125" style="1" customWidth="1"/>
+    <col min="6148" max="6400" width="11.42578125" style="1"/>
+    <col min="6401" max="6401" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6402" max="6402" width="28.5703125" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="57.42578125" style="1" customWidth="1"/>
+    <col min="6404" max="6656" width="11.42578125" style="1"/>
+    <col min="6657" max="6657" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6658" max="6658" width="28.5703125" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="57.42578125" style="1" customWidth="1"/>
+    <col min="6660" max="6912" width="11.42578125" style="1"/>
+    <col min="6913" max="6913" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6914" max="6914" width="28.5703125" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="57.42578125" style="1" customWidth="1"/>
+    <col min="6916" max="7168" width="11.42578125" style="1"/>
+    <col min="7169" max="7169" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7170" max="7170" width="28.5703125" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="57.42578125" style="1" customWidth="1"/>
+    <col min="7172" max="7424" width="11.42578125" style="1"/>
+    <col min="7425" max="7425" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7426" max="7426" width="28.5703125" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="57.42578125" style="1" customWidth="1"/>
+    <col min="7428" max="7680" width="11.42578125" style="1"/>
+    <col min="7681" max="7681" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7682" max="7682" width="28.5703125" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="57.42578125" style="1" customWidth="1"/>
+    <col min="7684" max="7936" width="11.42578125" style="1"/>
+    <col min="7937" max="7937" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7938" max="7938" width="28.5703125" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="57.42578125" style="1" customWidth="1"/>
+    <col min="7940" max="8192" width="11.42578125" style="1"/>
+    <col min="8193" max="8193" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8194" max="8194" width="28.5703125" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="57.42578125" style="1" customWidth="1"/>
+    <col min="8196" max="8448" width="11.42578125" style="1"/>
+    <col min="8449" max="8449" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8450" max="8450" width="28.5703125" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="57.42578125" style="1" customWidth="1"/>
+    <col min="8452" max="8704" width="11.42578125" style="1"/>
+    <col min="8705" max="8705" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8706" max="8706" width="28.5703125" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="57.42578125" style="1" customWidth="1"/>
+    <col min="8708" max="8960" width="11.42578125" style="1"/>
+    <col min="8961" max="8961" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8962" max="8962" width="28.5703125" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="57.42578125" style="1" customWidth="1"/>
+    <col min="8964" max="9216" width="11.42578125" style="1"/>
+    <col min="9217" max="9217" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9218" max="9218" width="28.5703125" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="57.42578125" style="1" customWidth="1"/>
+    <col min="9220" max="9472" width="11.42578125" style="1"/>
+    <col min="9473" max="9473" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9474" max="9474" width="28.5703125" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="57.42578125" style="1" customWidth="1"/>
+    <col min="9476" max="9728" width="11.42578125" style="1"/>
+    <col min="9729" max="9729" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9730" max="9730" width="28.5703125" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="57.42578125" style="1" customWidth="1"/>
+    <col min="9732" max="9984" width="11.42578125" style="1"/>
+    <col min="9985" max="9985" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9986" max="9986" width="28.5703125" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="57.42578125" style="1" customWidth="1"/>
+    <col min="9988" max="10240" width="11.42578125" style="1"/>
+    <col min="10241" max="10241" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10242" max="10242" width="28.5703125" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="57.42578125" style="1" customWidth="1"/>
+    <col min="10244" max="10496" width="11.42578125" style="1"/>
+    <col min="10497" max="10497" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10498" max="10498" width="28.5703125" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="57.42578125" style="1" customWidth="1"/>
+    <col min="10500" max="10752" width="11.42578125" style="1"/>
+    <col min="10753" max="10753" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10754" max="10754" width="28.5703125" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="57.42578125" style="1" customWidth="1"/>
+    <col min="10756" max="11008" width="11.42578125" style="1"/>
+    <col min="11009" max="11009" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11010" max="11010" width="28.5703125" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="57.42578125" style="1" customWidth="1"/>
+    <col min="11012" max="11264" width="11.42578125" style="1"/>
+    <col min="11265" max="11265" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11266" max="11266" width="28.5703125" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="57.42578125" style="1" customWidth="1"/>
+    <col min="11268" max="11520" width="11.42578125" style="1"/>
+    <col min="11521" max="11521" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11522" max="11522" width="28.5703125" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="57.42578125" style="1" customWidth="1"/>
+    <col min="11524" max="11776" width="11.42578125" style="1"/>
+    <col min="11777" max="11777" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11778" max="11778" width="28.5703125" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="57.42578125" style="1" customWidth="1"/>
+    <col min="11780" max="12032" width="11.42578125" style="1"/>
+    <col min="12033" max="12033" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12034" max="12034" width="28.5703125" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="57.42578125" style="1" customWidth="1"/>
+    <col min="12036" max="12288" width="11.42578125" style="1"/>
+    <col min="12289" max="12289" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12290" max="12290" width="28.5703125" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="57.42578125" style="1" customWidth="1"/>
+    <col min="12292" max="12544" width="11.42578125" style="1"/>
+    <col min="12545" max="12545" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12546" max="12546" width="28.5703125" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="57.42578125" style="1" customWidth="1"/>
+    <col min="12548" max="12800" width="11.42578125" style="1"/>
+    <col min="12801" max="12801" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12802" max="12802" width="28.5703125" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="57.42578125" style="1" customWidth="1"/>
+    <col min="12804" max="13056" width="11.42578125" style="1"/>
+    <col min="13057" max="13057" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13058" max="13058" width="28.5703125" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="57.42578125" style="1" customWidth="1"/>
+    <col min="13060" max="13312" width="11.42578125" style="1"/>
+    <col min="13313" max="13313" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13314" max="13314" width="28.5703125" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="57.42578125" style="1" customWidth="1"/>
+    <col min="13316" max="13568" width="11.42578125" style="1"/>
+    <col min="13569" max="13569" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13570" max="13570" width="28.5703125" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="57.42578125" style="1" customWidth="1"/>
+    <col min="13572" max="13824" width="11.42578125" style="1"/>
+    <col min="13825" max="13825" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13826" max="13826" width="28.5703125" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="57.42578125" style="1" customWidth="1"/>
+    <col min="13828" max="14080" width="11.42578125" style="1"/>
+    <col min="14081" max="14081" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14082" max="14082" width="28.5703125" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="57.42578125" style="1" customWidth="1"/>
+    <col min="14084" max="14336" width="11.42578125" style="1"/>
+    <col min="14337" max="14337" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14338" max="14338" width="28.5703125" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="57.42578125" style="1" customWidth="1"/>
+    <col min="14340" max="14592" width="11.42578125" style="1"/>
+    <col min="14593" max="14593" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14594" max="14594" width="28.5703125" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="57.42578125" style="1" customWidth="1"/>
+    <col min="14596" max="14848" width="11.42578125" style="1"/>
+    <col min="14849" max="14849" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14850" max="14850" width="28.5703125" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="57.42578125" style="1" customWidth="1"/>
+    <col min="14852" max="15104" width="11.42578125" style="1"/>
+    <col min="15105" max="15105" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15106" max="15106" width="28.5703125" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="57.42578125" style="1" customWidth="1"/>
+    <col min="15108" max="15360" width="11.42578125" style="1"/>
+    <col min="15361" max="15361" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15362" max="15362" width="28.5703125" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="57.42578125" style="1" customWidth="1"/>
+    <col min="15364" max="15616" width="11.42578125" style="1"/>
+    <col min="15617" max="15617" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15618" max="15618" width="28.5703125" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="57.42578125" style="1" customWidth="1"/>
+    <col min="15620" max="15872" width="11.42578125" style="1"/>
+    <col min="15873" max="15873" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15874" max="15874" width="28.5703125" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="57.42578125" style="1" customWidth="1"/>
+    <col min="15876" max="16128" width="11.42578125" style="1"/>
+    <col min="16129" max="16129" width="2.7109375" style="1" customWidth="1"/>
+    <col min="16130" max="16130" width="28.5703125" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="57.42578125" style="1" customWidth="1"/>
+    <col min="16132" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1833,21 +1869,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="11"/>
       <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
@@ -1859,79 +1895,79 @@
         <v>22</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="8"/>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20" t="s">
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="27"/>
+      <c r="B5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="19"/>
       <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="17"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="C7" s="26"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20" t="s">
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="25"/>
+      <c r="B11" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="19"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
@@ -1950,261 +1986,273 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="16" t="s">
+    <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="18">
         <f>SUM(H13:H31)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="8"/>
-      <c r="C33" s="14"/>
-    </row>
-    <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21" t="s">
+    <row r="33" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="7"/>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="20"/>
+      <c r="B34" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="21"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="11" t="s">
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="22"/>
+      <c r="B35" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="11" t="s">
+      <c r="C35" s="15"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="22"/>
+      <c r="B36" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
+      <c r="C36" s="15"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="22"/>
+      <c r="B37" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="11"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="11" t="s">
+      <c r="C37" s="15"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="22"/>
+      <c r="B38" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="11"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="11" t="s">
+      <c r="C38" s="15"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="22"/>
+      <c r="B39" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="11"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="11" t="s">
+      <c r="C39" s="15"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="22"/>
+      <c r="B40" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="11"/>
-    </row>
-    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20" t="s">
+      <c r="C40" s="15"/>
+    </row>
+    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="23"/>
+      <c r="B41" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="20"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="11" t="s">
+      <c r="C41" s="24"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="22"/>
+      <c r="B42" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="11"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="11" t="s">
+      <c r="C42" s="15"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="22"/>
+      <c r="B43" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="11"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="11" t="s">
+      <c r="C43" s="15"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C44" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="H2:H6"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C37">
@@ -2228,15 +2276,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Listo para revisión</Status>
@@ -2249,6 +2288,15 @@
     </Owner>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2336,14 +2384,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{862920E9-66EB-4C3E-957A-EA8E4211520C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2354,6 +2394,14 @@
     <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>